<commit_message>
some practices were added
</commit_message>
<xml_diff>
--- a/prac_7.xlsx
+++ b/prac_7.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="F Name" sheetId="2" r:id="rId2"/>
+    <sheet name="Total sal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
   <si>
     <t>S No</t>
   </si>
@@ -113,10 +113,19 @@
     <t>Raja</t>
   </si>
   <si>
-    <t>Trgt - Adding Table</t>
-  </si>
-  <si>
     <t>To add table (select insert tab\tables groupo\Table).</t>
+  </si>
+  <si>
+    <t>To add pictures (select insert tab\pictures)</t>
+  </si>
+  <si>
+    <t>to add shapes (select insert tab\shapes)</t>
+  </si>
+  <si>
+    <t>Hyperlinks are also added in two columns (in blue color).</t>
+  </si>
+  <si>
+    <t>Trgt - Adding Table, pictures &amp; shapes, Hyperlinks</t>
   </si>
 </sst>
 </file>
@@ -126,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +165,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +198,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor theme="5" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -291,10 +327,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -356,8 +396,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -605,6 +669,314 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>181523</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>117980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>349722</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>89337</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="image.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5393603" y="117980"/>
+          <a:ext cx="168199" cy="199957"/>
+        </a:xfrm>
+        <a:prstGeom prst="round2DiagRect">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16667"/>
+            <a:gd name="adj2" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="254000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>44931</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>112723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>213130</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>84080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="image.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1119351" y="112723"/>
+          <a:ext cx="168199" cy="199957"/>
+        </a:xfrm>
+        <a:prstGeom prst="round2DiagRect">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16667"/>
+            <a:gd name="adj2" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="254000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>154502</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180515</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Smiley Face 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3362522" y="3716195"/>
+          <a:ext cx="698938" cy="611965"/>
+        </a:xfrm>
+        <a:prstGeom prst="smileyFace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219929</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>46246</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>616695</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>77776</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Explosion 1 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4624289" y="4496326"/>
+          <a:ext cx="1082566" cy="1128810"/>
+        </a:xfrm>
+        <a:prstGeom prst="irregularSeal1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>545487</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>113249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>204952</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>150035</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Heart 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4584087" y="4929089"/>
+          <a:ext cx="299545" cy="219666"/>
+        </a:xfrm>
+        <a:prstGeom prst="heart">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -915,29 +1287,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="7.77734375" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:14" ht="18">
       <c r="A1" s="23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -949,11 +1321,16 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="3" spans="1:10" ht="15.6">
+    <row r="2" spans="1:14">
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.6">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
@@ -971,7 +1348,7 @@
       <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="37" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="21" t="s">
@@ -981,7 +1358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:14">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1011,11 +1388,11 @@
         <v>1300</v>
       </c>
       <c r="J4" s="11" t="str">
-        <f t="shared" ref="J4:J17" si="1">CONCATENATE(B4," ",C4)</f>
+        <f t="shared" ref="J4:L17" si="1">CONCATENATE(B4," ",C4)</f>
         <v>Ram Kumar</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:14">
       <c r="A5" s="10">
         <v>2</v>
       </c>
@@ -1049,7 +1426,7 @@
         <v>Gopal Verma</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:14">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -1083,7 +1460,7 @@
         <v>Joshef Paul</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:14">
       <c r="A7" s="10">
         <v>4</v>
       </c>
@@ -1117,7 +1494,7 @@
         <v>Hari Singh</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:14">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -1151,7 +1528,7 @@
         <v>Raja Ram</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:14">
       <c r="A9" s="9">
         <v>1</v>
       </c>
@@ -1185,7 +1562,7 @@
         <v>Ram Kumar</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:14">
       <c r="A10" s="10">
         <v>2</v>
       </c>
@@ -1219,7 +1596,7 @@
         <v>Gopal Verma</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:14">
       <c r="A11" s="10">
         <v>3</v>
       </c>
@@ -1253,7 +1630,7 @@
         <v>Joshef Paul</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:14">
       <c r="A12" s="10">
         <v>4</v>
       </c>
@@ -1287,7 +1664,7 @@
         <v>Hari Singh</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:14">
       <c r="A13" s="10">
         <v>5</v>
       </c>
@@ -1321,7 +1698,7 @@
         <v>Raja Ram</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:14">
       <c r="A14" s="10">
         <v>3</v>
       </c>
@@ -1355,7 +1732,7 @@
         <v>Joshef Paul</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:14">
       <c r="A15" s="10">
         <v>4</v>
       </c>
@@ -1389,7 +1766,7 @@
         <v>Hari Singh</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:14">
       <c r="A16" s="10">
         <v>5</v>
       </c>
@@ -1459,46 +1836,243 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
     </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="E29" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="L2:N2"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A22:E22"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B3" location="'F Name'!A1" display="Firs Name"/>
+    <hyperlink ref="H3" location="'Total sal'!A1" display="Sal Total"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Sheet2!A1" display="Firs Name"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.6">
+      <c r="A1" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="33">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="34">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="35">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="34">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="35">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="36">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="35">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="34">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="35">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="34">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="35">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="34">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="35">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="36">
+        <v>3900</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>